<commit_message>
Enclosure solidworks and 3D print files
</commit_message>
<xml_diff>
--- a/Bill of materials/Non-MFG BOM.xlsx
+++ b/Bill of materials/Non-MFG BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmerl\Documents\4th Year\ELEC491\repo\Group49\Bill of materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6419374A-05E3-4597-99B7-C91EF833E50F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EDEA76-3588-4545-8FD2-235A7431F118}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Part</t>
   </si>
@@ -60,9 +60,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Cost dependant on printing</t>
-  </si>
-  <si>
     <t>Electrodes</t>
   </si>
   <si>
@@ -103,6 +100,30 @@
   </si>
   <si>
     <t>Need both pickit and FTDI to program?</t>
+  </si>
+  <si>
+    <t>Battery 3</t>
+  </si>
+  <si>
+    <t>Li, 3.7V, 400mAh, 35.5x16.6x7.6mm</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3898</t>
+  </si>
+  <si>
+    <t>6.95USD</t>
+  </si>
+  <si>
+    <t>32 * 1.66 = 53 hr battery life</t>
+  </si>
+  <si>
+    <t>~32 hr battery life according to our estimates - we have this battery</t>
+  </si>
+  <si>
+    <t>32*0.33 = 10 hr battery life - optimal for reduced enclosure size</t>
+  </si>
+  <si>
+    <t>Cost dependant on printing, designed for small battery (Battery 2)</t>
   </si>
 </sst>
 </file>
@@ -440,16 +461,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -471,55 +492,61 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
+      <c r="E2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -528,29 +555,47 @@
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{B5E0C911-1FAD-49FB-BEAE-9CB9EFE7ABFC}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{B5E0C911-1FAD-49FB-BEAE-9CB9EFE7ABFC}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{F48FB37B-5661-4CF5-8A78-C96AF54AA5D2}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{B3521948-7653-4A88-ABDA-7D9B715BBEC1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>